<commit_message>
Main-Sheet umgezogen auf mehr Daten Stand 05.12.2025
</commit_message>
<xml_diff>
--- a/Projekt/Mitarbeiterzeiten/MA_KL.xlsx
+++ b/Projekt/Mitarbeiterzeiten/MA_KL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UBXGitHub\HtmXRechnung\Projekt\Mitarbeiterzeiten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBC31CF0-B27C-4D6C-B9E1-14E54CA0629C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA4EA31F-41A0-4264-8F34-70805C986475}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="22860" xr2:uid="{B876A782-0F35-4F50-9D0F-A8F7C1FEAC97}"/>
+    <workbookView xWindow="4800" yWindow="0" windowWidth="25575" windowHeight="18255" xr2:uid="{B876A782-0F35-4F50-9D0F-A8F7C1FEAC97}"/>
   </bookViews>
   <sheets>
     <sheet name="MA KL" sheetId="1" r:id="rId1"/>

</xml_diff>